<commit_message>
Made modifications for formatting json data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,24 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
-  <x:si>
-    <x:t>value</x:t>
-  </x:si>
-  <x:si>
-    <x:t>color</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#F7464A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>300</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#F73435</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
+  <x:si>
+    <x:t>name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>totalTime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>chair</x:t>
+  </x:si>
+  <x:si>
+    <x:t>table</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>microwave</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sofa</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -394,28 +400,70 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2">
+      <x:c r="B2" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="B3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0" t="s">
         <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>